<commit_message>
finish avi custom role feature
</commit_message>
<xml_diff>
--- a/HUGO-TARDY/newFeatures_ArtistIn.xlsx
+++ b/HUGO-TARDY/newFeatures_ArtistIn.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haga\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FreelanceWork\freelancerrepo\HUGO-TARDY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDF0D0C-AA06-4865-BE42-D7594426EF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="New Features" sheetId="1" r:id="rId1"/>
@@ -286,7 +285,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,7 +468,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,7 +504,7 @@
         <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9293A933-CA2C-9F63-348E-FC7ED228EC56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9293A933-CA2C-9F63-348E-FC7ED228EC56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -555,7 +554,7 @@
         <xdr:cNvPr id="17" name="Image 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57173431-55D3-174B-7190-CBEEC42A1969}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{57173431-55D3-174B-7190-CBEEC42A1969}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -605,7 +604,7 @@
         <xdr:cNvPr id="19" name="Image 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{786A0592-6696-1970-7FFC-D502A77A2F9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{786A0592-6696-1970-7FFC-D502A77A2F9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -627,7 +626,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21045467" y="666689"/>
+          <a:off x="22674322" y="3007118"/>
           <a:ext cx="2458389" cy="1529664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -655,7 +654,7 @@
         <xdr:cNvPr id="4" name="Image 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F9E44B4-2B9C-BB7C-3428-1F0D607320DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F9E44B4-2B9C-BB7C-3428-1F0D607320DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -705,7 +704,7 @@
         <xdr:cNvPr id="6" name="Image 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFA8577B-5AE9-BDC3-B05C-F6AE6592A560}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BFA8577B-5AE9-BDC3-B05C-F6AE6592A560}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -755,7 +754,7 @@
         <xdr:cNvPr id="8" name="Image 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B361A3B6-6E77-A118-6EA1-9E80FD91F16D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B361A3B6-6E77-A118-6EA1-9E80FD91F16D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,7 +804,7 @@
         <xdr:cNvPr id="10" name="Image 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DC03FF5-FBFB-77FC-11F3-F0605FAD436A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DC03FF5-FBFB-77FC-11F3-F0605FAD436A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -855,7 +854,7 @@
         <xdr:cNvPr id="12" name="Image 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0528E937-EB34-65F1-4D46-7F9FC8CD8482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0528E937-EB34-65F1-4D46-7F9FC8CD8482}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -905,7 +904,7 @@
         <xdr:cNvPr id="15" name="Image 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C729D83-BC9E-EEC0-B113-62448F05BFB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C729D83-BC9E-EEC0-B113-62448F05BFB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -955,7 +954,7 @@
         <xdr:cNvPr id="18" name="Image 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{605E8F69-2B0E-24E9-0959-B63D038E4A4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{605E8F69-2B0E-24E9-0959-B63D038E4A4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1005,7 +1004,7 @@
         <xdr:cNvPr id="21" name="Image 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A6C2607-F50D-EDD2-10DD-94E948E2BD0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A6C2607-F50D-EDD2-10DD-94E948E2BD0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1055,7 +1054,7 @@
         <xdr:cNvPr id="25" name="Image 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67F00A34-008E-59AD-F73D-D5FE602D69D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67F00A34-008E-59AD-F73D-D5FE602D69D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1105,7 +1104,7 @@
         <xdr:cNvPr id="27" name="Image 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D9DAB3-C3BE-47E1-E65D-18C9723A170F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07D9DAB3-C3BE-47E1-E65D-18C9723A170F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1155,7 +1154,7 @@
         <xdr:cNvPr id="5" name="Image 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCDDD99E-FD2E-7B9B-91B1-AFEC55AE3FC7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCDDD99E-FD2E-7B9B-91B1-AFEC55AE3FC7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1205,7 +1204,7 @@
         <xdr:cNvPr id="9" name="Image 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21E26115-8578-6B72-0D33-71D38A8C9817}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{21E26115-8578-6B72-0D33-71D38A8C9817}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,7 +1254,7 @@
         <xdr:cNvPr id="14" name="Image 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBE2B317-6A72-F980-2480-C0A2B9C9844A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FBE2B317-6A72-F980-2480-C0A2B9C9844A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1310,7 +1309,7 @@
         <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F53C4330-457D-8FA5-354D-153A8F7175FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F53C4330-457D-8FA5-354D-153A8F7175FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1359,7 @@
         <xdr:cNvPr id="5" name="Image 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5226BA8B-9288-5B87-7581-9B7F17BB804F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5226BA8B-9288-5B87-7581-9B7F17BB804F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1657,14 +1656,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="46.140625" style="3" customWidth="1"/>
@@ -1932,12 +1931,12 @@
     <row r="11" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" display="https://artistin.fr/service_post/" xr:uid="{48F94507-624F-423D-B0B7-164787E13B4B}"/>
-    <hyperlink ref="E5" r:id="rId2" display="https://artistin.fr/order/?pid=2777 " xr:uid="{EE17AA6E-3C9C-45D1-9677-351BD5860880}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{68CF6C7B-3ED9-4591-B847-E9408B4B9B5F}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{28D13F14-4751-4F19-8829-B87BAE569F87}"/>
-    <hyperlink ref="E9" r:id="rId5" display="https://artistin.fr/recruit/" xr:uid="{878F075D-BA94-4A0A-9BBB-2C04BD14B9DE}"/>
-    <hyperlink ref="E10" r:id="rId6" display="https://artistin.fr/forum/members/" xr:uid="{8C608613-9C25-4B1D-AE30-E7FFDF4496C7}"/>
+    <hyperlink ref="E4" r:id="rId1" display="https://artistin.fr/service_post/"/>
+    <hyperlink ref="E5" r:id="rId2" display="https://artistin.fr/order/?pid=2777 "/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E9" r:id="rId5" display="https://artistin.fr/recruit/"/>
+    <hyperlink ref="E10" r:id="rId6" display="https://artistin.fr/forum/members/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
@@ -1946,14 +1945,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01F1817-85A3-4377-A1E9-D2A3101FB741}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.85546875" customWidth="1"/>
     <col min="2" max="2" width="117.140625" customWidth="1"/>

</xml_diff>